<commit_message>
Added more specific conformity for column names. Added filter function to remove irrelevant column names
</commit_message>
<xml_diff>
--- a/Class List.xlsx
+++ b/Class List.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O150"/>
+  <dimension ref="A1:K132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,2520 +466,2144 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>MKT 460</t>
+          <t>MKT 300</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Nick armin</t>
+          <t>Alekha Malhotra</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ryan Weingarden</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Allison Jablonski</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Samantha Chin</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Hana Turkmani</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Sujay Rao</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Andy Majtara</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Brady Kraft</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Owen Davis Lee</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Martha Ramirez </t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>MKT 430</t>
+          <t>MKT 317</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nick armin</t>
+          <t>Alekha Malhotra</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ryan Weingarden</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Vibha Mahesha</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Hana Turkmani</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Lauren Cooper</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simran </t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ateendra Ghosh </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Martha Ramirez </t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Ateendra Ghosh</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Luke Boldman</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>GBL 385</t>
+          <t>MGT 315</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nick armin</t>
+          <t>Alekha Malhotra</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ipsa Patel</t>
+          <t>Brooke Dahlke</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Audrey Parks</t>
+          <t>Amanda Koczara</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>John Stabinsky</t>
+          <t>Max Resch</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Jennifer Bloch</t>
+          <t>Ella Krause</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Savvy baby</t>
+          <t>Sujay Rao</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Reese Ben-Ezra</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>grace joo</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Colleen Owens</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>MKT 416</t>
+          <t>STA 110</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nick armin</t>
+          <t>Alekha Malhotra</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SCM 303</t>
+          <t>ACC 202</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Yennah Kim</t>
+          <t>Ryan Weingarden</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rayna Rajkumar</t>
+          <t>Vibha Mahesha</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jacqueline Lee</t>
+          <t>Colleen Andrews</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Abhinaya Vyyuri</t>
+          <t>Andy Majtara</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dakarai Young</t>
+          <t>Brady Kraft</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Kruthik Pamidighantam</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Max Resch</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Ateendra Ghosh</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Vivian Martinez</t>
+          <t>Luke Boldman</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>MKT 317</t>
+          <t>PLS 320</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Yennah Kim</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Grace Joo</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Audrey Parks</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Joshua Hsu</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Jacqueline Lee</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Emily Jud</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Reghan Lanfear</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Reghan Lanfear</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Nitish Gupta</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Rahul Rao</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Max Resch</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Shreya Peddi</t>
+          <t>Ryan Weingarden</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>MKT 300</t>
+          <t>FI 311</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Yennah Kim</t>
+          <t>Ryan Weingarden</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Grace Joo</t>
+          <t>Brooke Dahlke</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ben Staebler</t>
+          <t>Vibha Mahesha</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Audrey Parks</t>
+          <t>Hana Turkmani</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Joshua Hsu</t>
+          <t>Andy Majtara</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vishnu  Patcheak </t>
+          <t>Reese Ben-Ezra</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Emily Jud</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Nick Newcomer</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Miles Manapat</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Abhinaya Vyyuri</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Sophie Yang</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Kruthik Pamidighantam</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Nitish Gupta</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>Vivian Martinez</t>
+          <t>Brady Kraft</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>MKT 250</t>
+          <t>MGT 409</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Yennah Kim</t>
+          <t>Jenny Song</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Grace Joo</t>
+          <t>Nitish Gupta</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rayna Rajkumar</t>
+          <t>Cherry Sun</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Jacqueline Lee</t>
+          <t>Ben Staebler</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vishnu  Patcheak </t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Simran Raichandani</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Miles Manapat</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Abhinaya Vyyuri</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Dakarai Young</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Sujay Rao</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Sophie Yang</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Ateendra Ghosh</t>
+          <t>John Stabinsky</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>IAH 208A</t>
+          <t>SCM 373</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Yennah Kim</t>
+          <t>Jenny Song</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily Jud </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>ITM 209</t>
+          <t>GBL 385</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Grace Joo</t>
+          <t>Jenny Song</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jacqueline Lee</t>
+          <t>Ella Krause</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Abhinaya Vyyuri</t>
+          <t>Cherry Sun</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sophie Yang</t>
+          <t>grace joo</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Vivian Martinez</t>
+          <t xml:space="preserve">Vishnu  Patcheak </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>ACC 201</t>
+          <t>SCM 474</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Grace Joo</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Joshua Hsu</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Alekha</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Miles Manapat</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Dakarai Young</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Sujay Rao</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Sophie Yang</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Ateendra Ghosh</t>
+          <t>Jenny Song</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>KOR 401</t>
+          <t>STT 200</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Grace Joo</t>
+          <t>Anagha</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>MTH 314</t>
+          <t>EC 201</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Srikar Kante</t>
+          <t>Anagha</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Joseph Dougherty</t>
+          <t>Matthew Welmerink</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CSE 431</t>
+          <t>CSE 260</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Srikar Kante</t>
+          <t>Anagha</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CSE 320</t>
+          <t>CSE 300</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Srikar Kante</t>
+          <t>Anagha</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>GBL 323</t>
+          <t>ISS 305</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Srikar Kante</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Dalaija Franklin</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Ankit Goyal</t>
+          <t>Anagha</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>ACC 341</t>
+          <t>ADV 205</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chloe McKenzie </t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Mike McCarthy</t>
+          <t>Allison Jablonski</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>ACC 308</t>
+          <t>ACC 201</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chloe McKenzie </t>
+          <t>Allison Jablonski</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mike McCarthy</t>
+          <t>Samantha Chin</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Matthew Welmerink</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Owen Davis Lee</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>COM 875</t>
+          <t>ISP 203A</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chloe McKenzie </t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Mike McCarthy</t>
+          <t>Allison Jablonski</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>CEP 261</t>
+          <t>ISP 203L</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chloe McKenzie </t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Sujay Rao</t>
+          <t>Allison Jablonski</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MGT 409</t>
+          <t>BUS 100</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chloe McKenzie </t>
+          <t>Allison Jablonski</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Natalie Haight</t>
+          <t>Kayleigh Sleeper</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Jennifer Bloch</t>
+          <t>Owen Davis Lee</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Jill Umin</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Amanda murrell</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>John Biberstein</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Savvy baby</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Reilly Cannaday</t>
+          <t>Sneha Thodla</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>COM 275</t>
+          <t>MKT 891</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ashley Kim</t>
+          <t xml:space="preserve">Jillian Dempsey </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CJ 220</t>
+          <t>MKT 805</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ashley Kim</t>
+          <t xml:space="preserve">Jillian Dempsey </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Shravya Ramesh</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>PSY 491</t>
+          <t>MKT 816</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ashley Kim</t>
+          <t xml:space="preserve">Jillian Dempsey </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Shravya Ramesh</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>ENG 342</t>
+          <t>MKT 880</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ashley Kim</t>
+          <t xml:space="preserve">Jillian Dempsey </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>HDFS 212</t>
+          <t>CMSE 382</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Ashley Kim</t>
+          <t>Joseph Dougherty</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>IBUS 310</t>
+          <t>CSE 404</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jillian Dempsey</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Ben Staebler</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>John Stabinsky</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Emily Jud</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Hannah Bagaric</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Jenny Song</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Nitish Gupta</t>
+          <t>Joseph Dougherty</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>ISP 205</t>
+          <t>CSE 480</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jillian Dempsey</t>
+          <t>Joseph Dougherty</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>ISP 205L</t>
+          <t>MKT 327</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Jillian Dempsey</t>
+          <t>Joseph Dougherty</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ashley Kim</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Lana Nehme</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>trayza haido</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>ANP 225</t>
+          <t>REL 150</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jillian Dempsey</t>
+          <t>Joseph Dougherty</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>FI 311</t>
+          <t>MKT 313</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Jillian Dempsey</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Hannah Bagaric</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Jenny Song</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Sujay Rao</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Nitish Gupta</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Shreya Peddi</t>
+          <t>Brooke Dahlke</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>ACC 202</t>
+          <t>MKT 319</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Alyse Belkin</t>
+          <t>Brooke Dahlke</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Rayna Rajkumar</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Jacqueline Lee</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Vishnu  Patcheak </t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Reghan Lanfear</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Vivian Martinez</t>
+          <t>grace joo</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>GBL 386</t>
+          <t>IBUS 310</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Alyse Belkin</t>
+          <t>Brooke Dahlke</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Amanda Koczara</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Vibha Mahesha</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Sujay Rao</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Reese Ben-Ezra</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Lauren Cooper</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Colleen Owens</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Ateendra Ghosh</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vishnu  Patcheak </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>REL 175</t>
+          <t>IAH 209</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Alyse Belkin</t>
+          <t>Nick Carlisle</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nicholas Carlisle </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Sneha Thodla</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>FI 312</t>
+          <t>CMSE 202</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Alyse Belkin</t>
+          <t>Nick Carlisle</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ben Staebler</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Elise Rodriguez</t>
+          <t xml:space="preserve">Nicholas Carlisle </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>SOC 452</t>
+          <t>MTH 234</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Alyse Belkin</t>
+          <t>Nick Carlisle</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Elise Rodriguez</t>
+          <t xml:space="preserve">Nicholas Carlisle </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>HRLR 465</t>
+          <t>PHY 183</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Dalaija Franklin</t>
+          <t>Nick Carlisle</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nicholas Carlisle </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>CEP 470</t>
+          <t>ITM 209</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Dalaija Franklin</t>
+          <t>Samantha Chin</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Owen Davis Lee</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>PHL 340</t>
+          <t>CMSE 201</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Dalaija Franklin</t>
+          <t>Samantha Chin</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Andy Majtara</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>PSY 280</t>
+          <t>MKT 250</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Dalaija Franklin</t>
+          <t>Samantha Chin</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Simran Raichandani</t>
+          <t>Colleen Andrews</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Matthew Welmerink</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Brady Kraft</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Owen Davis Lee</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>MGT 315</t>
+          <t>EC 202</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ipsa Patel</t>
+          <t>Kayleigh Sleeper</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ben Staebler</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Joshua Hsu</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Emily Jud</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Joey DeRose</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Simran Raichandani</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Jenny Song</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>Nitish Gupta</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>Cherry Sun</t>
+          <t>Sneha Thodla</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SCM 371</t>
+          <t>IAH 231B</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ipsa Patel</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Sid Guruvi</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Audrey Parks</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Emily Jud</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Rahul Rao</t>
+          <t>Kayleigh Sleeper</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>ACM 271</t>
+          <t>ISP 203B</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Ipsa Patel</t>
+          <t>Kayleigh Sleeper</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Matthew Welmerink</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>CSUS 200</t>
+          <t>ISS 215</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ipsa Patel</t>
+          <t>Kayleigh Sleeper</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Dakarai Young</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Sophia Yee</t>
+          <t>Siya Vesikar</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>KIN 106</t>
+          <t>SCM 303</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mike McCarthy</t>
+          <t>Amanda Koczara</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Colleen Andrews</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Cherry Sun</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Lauren Cooper</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Luke Boldman</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>FI 801</t>
+          <t>MGT 412</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Mike McCarthy</t>
+          <t>Amanda Koczara</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>EC 425</t>
+          <t>MGT 413</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Samuel Stebbins</t>
+          <t>Amanda Koczara</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>FI 414</t>
+          <t>MC 321</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Samuel Stebbins</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Max Resch</t>
+          <t>Reagan Winnie</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>ACC 305</t>
+          <t>EC 302</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Samuel Stebbins</t>
+          <t>Reagan Winnie</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>FI 355</t>
+          <t>CSE 102</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Samuel Stebbins</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Kruthik Pamidighantam</t>
+          <t>Reagan Winnie</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>SCM 372</t>
+          <t>MC 361</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sid Guruvi</t>
+          <t>Reagan Winnie</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>SCM 373</t>
+          <t>CEM 161</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sid Guruvi</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Matt Moreau</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Sophia Yee</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Rahul Rao</t>
+          <t>Madelynn Frendo</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>ANP 370</t>
+          <t>CEM 142</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Sid Guruvi</t>
+          <t>Madelynn Frendo</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>GRM 455</t>
+          <t>CEM 251</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ben Staebler</t>
+          <t>Madelynn Frendo</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>CSE 102</t>
+          <t>ISB 202</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Rayna Rajkumar</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Luke Boldman</t>
+          <t>Madelynn Frendo</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>ISB 204</t>
+          <t>BS 182H</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Victoria Locricchio</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Rayna Rajkumar</t>
+          <t>Madelynn Frendo</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>ESHP 170</t>
+          <t>CSE 840</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Audrey Parks</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Matt Moreau</t>
+          <t>Max Resch</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MKT 302</t>
+          <t>CSE 498</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Natalie Haight</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Jennifer Bloch</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Hannah Bagaric</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Jenny Song</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Reghan Lanfear</t>
+          <t>Max Resch</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MKT 313</t>
+          <t>FI 853</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Natalie Haight</t>
+          <t>Max Resch</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Hannah Bagaric</t>
+          <t>Cherry Sun</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>HST 335</t>
+          <t>THR 350</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Matt Moreau</t>
+          <t>Max Resch</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>SCM 475</t>
+          <t>CSE 232</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Matt Moreau</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Sophia Yee</t>
+          <t>Vibha Mahesha</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>IAH 206</t>
+          <t>CSS 202</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Joshua Hsu</t>
+          <t>Nitish Gupta</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Luke Boldman</t>
+          <t>Shravya Ramesh</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>EC 330</t>
+          <t>FOR 360</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Ankit Goyal</t>
+          <t>Nitish Gupta</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MTH 124</t>
+          <t>GEO 330</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ankit Goyal</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>John Stabinsky</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Vivian Martinez</t>
+          <t>Nitish Gupta</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>FI 320</t>
+          <t>FI 460</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Ankit Goyal</t>
+          <t>Nitish Gupta</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>EC 302</t>
+          <t>ACC 300</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Ankit Goyal</t>
+          <t>Nitish Gupta</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>CJ 110</t>
+          <t>SPN 102</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ankit Goyal</t>
+          <t>Colleen Andrews</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MGT 475</t>
+          <t>CJ 210</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Kaitlyn Mather</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Elise Rodriguez</t>
+          <t>Colleen Andrews</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>MGT 413</t>
+          <t>ACC 305</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Kaitlyn Mather</t>
+          <t>Ella Krause</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simran </t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Colleen Owens</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vishnu  Patcheak </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>GBL 480</t>
+          <t>FRN 420</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Kaitlyn Mather</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Elise Rodriguez</t>
+          <t>Ella Krause</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>CSE 232</t>
+          <t>FI 312</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Joseph Dougherty</t>
+          <t>Ella Krause</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Hana Turkmani</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simran </t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Colleen Owens</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Abhinaya Vyyuri</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vishnu  Patcheak </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>STT 380</t>
+          <t>PSY 395</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Joseph Dougherty</t>
+          <t>Siya Vesikar</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>ENT 205</t>
+          <t>HRLR 211</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Joseph Dougherty</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Simran Raichandani</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Sophie Yang</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Reilly Cannaday</t>
+          <t>Siya Vesikar</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>CSE 300</t>
+          <t>PSY 491</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Joseph Dougherty</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Max Resch</t>
+          <t>Siya Vesikar</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>EC 201</t>
+          <t>FI 320</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Alekha</t>
+          <t>Siya Vesikar</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Luke Boldman</t>
+          <t>Ashley Kim</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>ISS 328</t>
+          <t>ISS 308</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Alekha</t>
+          <t>Matthew Welmerink</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>ISP 203B</t>
+          <t>GEO 435</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Alekha</t>
+          <t>Hana Turkmani</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>ISP 203L</t>
+          <t>GBL 323</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Alekha</t>
+          <t>Ashley Kim</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>ACC 300</t>
+          <t>MGT 325</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>John Stabinsky</t>
+          <t>Ashley Kim</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Joey DeRose</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Kruthik Pamidighantam</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Cherry Sun</t>
+          <t>victoria locricchio</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>ACC 321</t>
+          <t>SCM 304</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>John Stabinsky</t>
+          <t>Ashley Kim</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>ITM 209 TA</t>
+          <t>SCM 371</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Emily Jud</t>
+          <t>Sujay Rao</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ateendra Ghosh </t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Martha Ramirez </t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Ateendra Ghosh</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>ANTR 350</t>
+          <t>ESHP 190</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Briggs Hehl</t>
+          <t>Sujay Rao</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Riya Kapadia</t>
+          <t xml:space="preserve">Ateendra Ghosh </t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Ateendra Ghosh</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>PHL 462</t>
+          <t>HDFS 225</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Briggs Hehl</t>
+          <t xml:space="preserve">Emily Jud </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>PHM 431</t>
+          <t>SCM 463</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Briggs Hehl</t>
+          <t xml:space="preserve">Emily Jud </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>NEU 311</t>
+          <t>SOC 452</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Briggs Hehl</t>
+          <t xml:space="preserve">Emily Jud </t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>FI 413</t>
+          <t>CSUS 265</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Nick Newcomer</t>
+          <t xml:space="preserve">Emily Jud </t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Lauren Cooper</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>IAH 207</t>
+          <t>MGT 225</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Nick Newcomer</t>
+          <t>Andy Majtara</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Shreya Peddi</t>
+          <t>Brady Kraft</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CSE 331</t>
+          <t>ANP 200</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Nick Newcomer</t>
+          <t>Cherry Sun</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ateendra Ghosh </t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Ateendra Ghosh</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>ACC 250</t>
+          <t>FI 451</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Joey DeRose</t>
+          <t>Cherry Sun</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>HRLR 211</t>
+          <t>ADV 225</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Joey DeRose</t>
+          <t>Lana Nehme</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>ANP 201</t>
+          <t>CAS 110</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Joey DeRose</t>
+          <t>Lana Nehme</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>CEM 251</t>
+          <t>PR 330</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Riya Kapadia</t>
+          <t>Lana Nehme</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Lauren Cooper</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>MMG 302</t>
+          <t>MKT 806</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Riya Kapadia</t>
+          <t>Shravya Ramesh</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>PHY 221</t>
+          <t>MKT 861</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Riya Kapadia</t>
+          <t>Shravya Ramesh</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>MMG 301</t>
+          <t>MKT 867</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Riya Kapadia</t>
+          <t>Shravya Ramesh</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>PSL 101</t>
+          <t>AC 201</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Riya Kapadia</t>
+          <t>Reese Ben-Ezra</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MKT 300H</t>
+          <t>HB 105</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Simran Raichandani</t>
+          <t>Reese Ben-Ezra</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>ISS 220</t>
+          <t>NEU 301</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Miles Manapat</t>
+          <t>Victoria Nweze</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>HST 251</t>
+          <t>ISS 330 B</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Miles Manapat</t>
+          <t>Victoria Nweze</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>GRM 101</t>
+          <t>PSY 101</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Abhinaya Vyyuri</t>
+          <t>Victoria Nweze</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>EC 202</t>
+          <t>BS 171</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Victoria Locricchio</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Nicole Miciuda</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Ateendra Ghosh</t>
+          <t>Victoria Nweze</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>IAH 231</t>
+          <t>CEM 252</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Nicole Miciuda</t>
+          <t>Victoria Nweze</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>ISS 310</t>
+          <t>ACC 331</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Victoria Locricchio</t>
+          <t>Joey DeRose</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Nicole Miciuda</t>
+          <t>John Stabinsky</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>HDFS 138</t>
+          <t>HB 470</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Nicole Miciuda</t>
+          <t>Joey DeRose</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>ANP 203</t>
+          <t>HB 472</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Dakarai Young</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Ateendra Ghosh</t>
+          <t>Joey DeRose</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>RUS 201</t>
+          <t>HB 474</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Jennifer Bloch</t>
+          <t>Joey DeRose</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>RUS 231</t>
+          <t>HRLR 314</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Jennifer Bloch</t>
+          <t>Joey DeRose</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>victoria locricchio</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>GEO 435</t>
+          <t>HB 282</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Hannah Bagaric</t>
+          <t>Joey DeRose</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>ACC 301</t>
+          <t>FI 457</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Jill Umin</t>
+          <t>Brady Kraft</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>ACC 331</t>
+          <t>MKT 355</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Jill Umin</t>
+          <t>grace joo</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>HDFS 238</t>
+          <t>MKT 460</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Jill Umin</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Amanda murrell</t>
+          <t>grace joo</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>WS 103</t>
+          <t>HDFS 238</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Jill Umin</t>
+          <t xml:space="preserve">Simran </t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>MGT 460</t>
+          <t>IBUS 300</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Elise Rodriguez</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Savvy baby</t>
+          <t xml:space="preserve">Ateendra Ghosh </t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MKT 327</t>
+          <t>IAH 211A</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Elizabeth Sharkevich</t>
+          <t>Owen Davis Lee</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>PLS 351</t>
+          <t>HRLR 420</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Elizabeth Sharkevich</t>
+          <t>victoria locricchio</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>ME 361</t>
+          <t>HRLR 316</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Elizabeth Sharkevich</t>
+          <t>victoria locricchio</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>MSE 250</t>
+          <t>HRLR 493</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Elizabeth Sharkevich</t>
+          <t>victoria locricchio</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>ME 280</t>
+          <t>ME 201</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Elizabeth Sharkevich</t>
+          <t>trayza haido</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>ME 391</t>
+          <t>ME 222</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Elizabeth Sharkevich</t>
+          <t>trayza haido</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>SCAM 474</t>
+          <t>MSE 250</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Amanda murrell</t>
+          <t>trayza haido</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MUS 175</t>
+          <t>UGS 201</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Amanda murrell</t>
+          <t>trayza haido</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>SCM 470</t>
+          <t>UGS 292</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Amanda murrell</t>
+          <t>trayza haido</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>MKT 319</t>
+          <t>IBUS 311</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Jenny Song</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Reghan Lanfear</t>
+          <t xml:space="preserve">Martha Ramirez </t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>FI 853</t>
+          <t>FI 355</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>John Biberstein</t>
+          <t>Ben Staebler</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Abhinaya Vyyuri</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vishnu  Patcheak </t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>FSC 211</t>
+          <t>FI 414</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>John Biberstein</t>
+          <t>Ben Staebler</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Abhinaya Vyyuri</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>FI 491</t>
+          <t>GEO 203</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>John Biberstein</t>
+          <t>Ben Staebler</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>IAH 208</t>
+          <t>FI 413</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Victoria Locricchio</t>
+          <t>Abhinaya Vyyuri</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>ISP 203</t>
+          <t>ISS 205</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Victoria Locricchio</t>
+          <t>Sneha Thodla</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>MGT 412</t>
+          <t>ISB 204</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Savvy baby</t>
+          <t>Sneha Thodla</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>MGT 491</t>
+          <t>ACC 341</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Savvy baby</t>
+          <t>John Stabinsky</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>YOUR MOM 101</t>
+          <t>CSE 231</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Savvy baby</t>
+          <t>John Stabinsky</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>HB 470</t>
+          <t>ITM 311</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Kruthik Pamidighantam</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="2" t="inlineStr">
-        <is>
-          <t>FI 844</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>Cherry Sun</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="2" t="inlineStr">
-        <is>
-          <t>FI 862</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>Cherry Sun</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Reilly Cannaday</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="2" t="inlineStr">
-        <is>
-          <t>FI 491- 004</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Cherry Sun</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="2" t="inlineStr">
-        <is>
-          <t>SCM 474</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>Sophia Yee</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="2" t="inlineStr">
-        <is>
-          <t>MI 480</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>Sophia Yee</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="2" t="inlineStr">
-        <is>
-          <t>FRN 330</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>Rahul Rao</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="2" t="inlineStr">
-        <is>
-          <t>CSE 480</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Max Resch</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="2" t="inlineStr">
-        <is>
-          <t>CSE 325</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>Max Resch</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="2" t="inlineStr">
-        <is>
-          <t>CAS 114</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Ateendra Ghosh</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="2" t="inlineStr">
-        <is>
-          <t>CSUS 265</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>Shreya Peddi</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="2" t="inlineStr">
-        <is>
-          <t>ADV 442</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>Kristen Lenz</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="2" t="inlineStr">
-        <is>
-          <t>CAS 110</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>Kristen Lenz</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="2" t="inlineStr">
-        <is>
-          <t>ADV 225</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>Kristen Lenz</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="2" t="inlineStr">
-        <is>
-          <t>ACC 230</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>Kristen Lenz</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="2" t="inlineStr">
-        <is>
-          <t>ADV 375</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>Kristen Lenz</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="2" t="inlineStr">
-        <is>
-          <t>FI 491 004</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Reilly Cannaday</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="2" t="inlineStr">
-        <is>
-          <t>PSY 101</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Reilly Cannaday</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="2" t="inlineStr">
-        <is>
-          <t>ANP 455</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>Reilly Cannaday</t>
+          <t>John Stabinsky</t>
         </is>
       </c>
     </row>

</xml_diff>